<commit_message>
Add toss delivery splitting settings and update the version.
</commit_message>
<xml_diff>
--- a/tests/excel_examples/devliery_confirmations.xlsx
+++ b/tests/excel_examples/devliery_confirmations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunyoungyoo/Projects/dotori/tests/excel_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA30E5DE-2281-2149-8291-C1C50561C86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7A77C7-5637-DF46-888F-2B83CC19CBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2300" yWindow="2540" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="149">
   <si>
     <t>NO</t>
   </si>
@@ -426,6 +426,55 @@
   </si>
   <si>
     <t>20241010878934705</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>623959232870</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1023811721</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9691126363</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>토스트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>경상도 구미시 불고기구 쌈장동</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6개월 세트(재사용 가능 필터본품 1개+리필주머니 6개)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>무인택배함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024070568997150</t>
+  </si>
+  <si>
+    <t>2024070568997151</t>
+  </si>
+  <si>
+    <t>2024070568997152</t>
+  </si>
+  <si>
+    <t>2024070568997153</t>
+  </si>
+  <si>
+    <t>2024070568997154</t>
+  </si>
+  <si>
+    <t>2024070568997155</t>
   </si>
 </sst>
 </file>
@@ -433,7 +482,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -510,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -532,12 +581,11 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -845,8 +893,8 @@
   </sheetPr>
   <dimension ref="A1:AV21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF14" sqref="AF14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -1037,8 +1085,8 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="9">
-        <v>2024070568997150</v>
+      <c r="J2" s="8" t="s">
+        <v>143</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>52</v>
@@ -1119,8 +1167,8 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="9">
-        <v>2024070568997151</v>
+      <c r="J3" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>52</v>
@@ -1201,8 +1249,8 @@
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="9">
-        <v>2024070568997152</v>
+      <c r="J4" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>52</v>
@@ -1283,8 +1331,8 @@
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="9">
-        <v>2024070568997153</v>
+      <c r="J5" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>52</v>
@@ -1360,8 +1408,8 @@
       <c r="G6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="10">
-        <v>2024070568997154</v>
+      <c r="J6" s="8" t="s">
+        <v>147</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>52</v>
@@ -1431,8 +1479,8 @@
       <c r="G7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J7" s="10">
-        <v>2024070568997155</v>
+      <c r="J7" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>52</v>
@@ -1502,7 +1550,7 @@
       <c r="G8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>86</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -1570,7 +1618,7 @@
       <c r="G9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>6950051903</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -1638,7 +1686,7 @@
       <c r="G10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>7604361881</v>
       </c>
       <c r="K10" s="2" t="s">
@@ -1706,7 +1754,7 @@
       <c r="G11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>7444642307</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1774,7 +1822,7 @@
       <c r="G12" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="9">
         <v>70472234126074</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1845,7 +1893,7 @@
       <c r="G13" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="9">
         <v>59645562145217</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1916,7 +1964,7 @@
       <c r="G14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="10" t="s">
         <v>133</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -1985,7 +2033,7 @@
       <c r="G15" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="11" t="s">
         <v>134</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -2038,8 +2086,100 @@
       </c>
     </row>
     <row r="16" spans="1:48" ht="17.25" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="S16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="T16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="U16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="V16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="W16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="X16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD16" s="12"/>
+      <c r="AE16" s="12"/>
+      <c r="AF16" s="12"/>
+      <c r="AG16" s="12"/>
+      <c r="AH16" s="12"/>
+      <c r="AI16" s="12"/>
+      <c r="AJ16" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="AK16" s="12"/>
+      <c r="AL16" s="12"/>
+      <c r="AM16" s="12"/>
+      <c r="AN16" s="12">
+        <v>1</v>
+      </c>
+      <c r="AO16" s="12"/>
+      <c r="AP16" s="12"/>
+      <c r="AQ16" s="12"/>
+      <c r="AR16" s="12"/>
+      <c r="AS16" s="12"/>
+      <c r="AT16" s="12"/>
+      <c r="AU16" s="12"/>
+      <c r="AV16" s="12"/>
     </row>
     <row r="17" spans="1:7" ht="17.25" customHeight="1">
       <c r="A17" s="5"/>

</xml_diff>